<commit_message>
limited to only instance of the application running at a time
</commit_message>
<xml_diff>
--- a/results table/results.xlsx
+++ b/results table/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Custom AI Model</t>
+          <t>Naive Bayes</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -468,16 +468,136 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PCA</t>
+          <t>No Technique</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Custom AI Model</t>
+          <t>Naive Bayes</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.933249791144528</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Naive Bayes</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Naive Bayes</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.9665831244778612</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Naive Bayes</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.9665831244778612</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.9665831244778612</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>No Technique</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.9665831244778612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed something on the grid-search
</commit_message>
<xml_diff>
--- a/results table/results.xlsx
+++ b/results table/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,36 @@
           <t>F1-Score</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Processing Time</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ROC AUC</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Memory Usage</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,11 +488,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>Naive Bayes</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7916666666666666</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0206162929534912</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5703125</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -473,11 +521,29 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.8997493734335839</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.009204864501953101</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +558,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.8329156223893066</v>
+        <v>0.9665831244778612</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1120295524597168</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9933333333333332</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.88671875</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9696969696969696</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9666666666666668</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9666666666666668</v>
       </c>
     </row>
     <row r="5">
@@ -503,11 +587,29 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>DecisionTree</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8329156223893065</v>
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0281538963317871</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.7734375</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -518,11 +620,29 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>RandomForest</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9665831244778612</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2764220237731933</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.5625</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -533,11 +653,29 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>KNN</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9326599326599326</v>
+        <v>0.9665831244778612</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0200996398925781</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.78125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.9696969696969696</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9666666666666668</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.9666666666666668</v>
       </c>
     </row>
     <row r="8">
@@ -548,11 +686,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>LogReg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.8950004244121891</v>
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0265321731567382</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +719,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>GradientBoost</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.8997493734335839</v>
+        <v>0.9665831244778612</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1955735683441162</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.9741666666666668</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.12890625</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.9696969696969696</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9666666666666668</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.9666666666666668</v>
       </c>
     </row>
     <row r="10">
@@ -578,11 +752,29 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>XGBoost</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.8981620718462824</v>
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.077242374420166</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.50390625</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -593,11 +785,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>Custom AI Model</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8</v>
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0213708877563476</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.7109375</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>